<commit_message>
references for Ex. Appendix
</commit_message>
<xml_diff>
--- a/data/hM_trial.xlsx
+++ b/data/hM_trial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinschuman/Documents/github/MaterialExergyPaper/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C329899-C20C-E94D-950D-B1BF64B45056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24755088-3794-BC48-805B-F4E0476B63FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="3020" windowWidth="37700" windowHeight="23360" activeTab="2" xr2:uid="{60ED9AA8-3852-9842-B346-E2FD5CB3AA75}"/>
+    <workbookView xWindow="6400" yWindow="800" windowWidth="37700" windowHeight="23360" activeTab="2" xr2:uid="{60ED9AA8-3852-9842-B346-E2FD5CB3AA75}"/>
   </bookViews>
   <sheets>
     <sheet name="h" sheetId="2" r:id="rId1"/>
@@ -1541,8 +1541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE18B6-B8F5-6345-9BBC-83B29165D6F4}">
   <dimension ref="A1:BM84"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75:I76"/>
+    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7654,7 +7654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06264013-ABCC-9745-870A-4E82469D68A7}">
   <dimension ref="B1:BX231"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
+    <sheetView topLeftCell="D79" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
@@ -18445,11 +18445,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="AQ37:BE37"/>
-    <mergeCell ref="BK37:BX37"/>
-    <mergeCell ref="AQ76:BE76"/>
-    <mergeCell ref="AQ116:BE116"/>
-    <mergeCell ref="BK116:BL116"/>
     <mergeCell ref="C165:K165"/>
     <mergeCell ref="C206:G206"/>
     <mergeCell ref="AQ118:BE118"/>
@@ -18458,6 +18453,11 @@
     <mergeCell ref="C138:AK138"/>
     <mergeCell ref="C159:AK159"/>
     <mergeCell ref="C161:AK161"/>
+    <mergeCell ref="AQ37:BE37"/>
+    <mergeCell ref="BK37:BX37"/>
+    <mergeCell ref="AQ76:BE76"/>
+    <mergeCell ref="AQ116:BE116"/>
+    <mergeCell ref="BK116:BL116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18467,8 +18467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{817C05AA-D3A9-6049-AB59-84B5F03A5DC4}">
   <dimension ref="B1:BO154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="Q115" sqref="Q115"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L144" sqref="L144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30650,16 +30650,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E82:AM82"/>
+    <mergeCell ref="E84:AM84"/>
+    <mergeCell ref="E95:M95"/>
+    <mergeCell ref="E136:I136"/>
+    <mergeCell ref="AS40:BG40"/>
     <mergeCell ref="BM40:BN40"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="AS42:BG42"/>
     <mergeCell ref="E59:AM59"/>
     <mergeCell ref="E61:AM61"/>
-    <mergeCell ref="E82:AM82"/>
-    <mergeCell ref="E84:AM84"/>
-    <mergeCell ref="E95:M95"/>
-    <mergeCell ref="E136:I136"/>
-    <mergeCell ref="AS40:BG40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>